<commit_message>
I am updating my code............
</commit_message>
<xml_diff>
--- a/DataDrivenFramework/XLData/TestData.xlsx
+++ b/DataDrivenFramework/XLData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="15735" windowHeight="6345"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="16785" windowHeight="6330"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="11">
   <si>
     <t>Shubham</t>
   </si>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t>George@2580</t>
+  </si>
+  <si>
+    <t>skv</t>
+  </si>
+  <si>
+    <t>shubham</t>
   </si>
 </sst>
 </file>
@@ -389,10 +395,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -407,6 +413,22 @@
       </c>
       <c r="B1" s="2" t="s">
         <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>